<commit_message>
some minor updates, and additional information for each recording
</commit_message>
<xml_diff>
--- a/Other_workbooks/wholeCellSTPCellList.xlsx
+++ b/Other_workbooks/wholeCellSTPCellList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\glickfeld_lab\Documents\docubase\Other_workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charlie\Documents\SourceTree_local\docubase\Other_workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="263">
   <si>
     <t>Mouse Name</t>
   </si>
@@ -771,6 +771,48 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>CH_160507_B</t>
+  </si>
+  <si>
+    <t>2016_06_06_0000</t>
+  </si>
+  <si>
+    <t>2016_06_06_0001</t>
+  </si>
+  <si>
+    <t>concat_2016_06_06_2to4</t>
+  </si>
+  <si>
+    <t>19:21, 77:98</t>
+  </si>
+  <si>
+    <t>-28, 20</t>
+  </si>
+  <si>
+    <t>-29,17</t>
+  </si>
+  <si>
+    <t>36, -356</t>
+  </si>
+  <si>
+    <t>Cell type1</t>
+  </si>
+  <si>
+    <t>Cell type 2</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>NPVIN</t>
   </si>
 </sst>
 </file>
@@ -1148,11 +1190,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1165,20 +1207,21 @@
     <col min="6" max="6" width="11.28515625" style="3" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="3" customWidth="1"/>
     <col min="8" max="9" width="6.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="8" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="7" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="35.85546875" style="5" customWidth="1"/>
-    <col min="20" max="16384" width="19" style="3"/>
+    <col min="10" max="11" width="8.140625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="8" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="7" style="3" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="8.5703125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="35.85546875" style="5" customWidth="1"/>
+    <col min="22" max="16384" width="19" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1207,37 +1250,43 @@
         <v>5</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1259,23 +1308,26 @@
       <c r="I2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1300,29 +1352,32 @@
       <c r="I3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="S3" s="5" t="s">
+      <c r="U3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -1347,26 +1402,29 @@
       <c r="I4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="5" t="s">
+      <c r="U4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1389,31 +1447,37 @@
         <v>19</v>
       </c>
       <c r="J5" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="R5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="5" t="s">
+      <c r="U5" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1436,31 +1500,37 @@
         <v>19</v>
       </c>
       <c r="J6" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="R6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="U6" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>59</v>
       </c>
@@ -1482,29 +1552,32 @@
       <c r="I7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="R7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Q7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>59</v>
       </c>
@@ -1526,29 +1599,32 @@
       <c r="I8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="K8" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="R8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="S8" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>73</v>
       </c>
@@ -1570,32 +1646,35 @@
       <c r="I9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="K9" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="M9" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="N9" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="R9" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>73</v>
       </c>
@@ -1618,31 +1697,37 @@
         <v>19</v>
       </c>
       <c r="J10" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>86</v>
       </c>
@@ -1668,34 +1753,40 @@
         <v>19</v>
       </c>
       <c r="J11" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="N11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="R11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q11" s="3" t="s">
+      <c r="S11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S11" s="5" t="s">
+      <c r="U11" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>95</v>
       </c>
@@ -1720,29 +1811,32 @@
       <c r="I12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L12" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="N12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="O12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="Q12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P12" s="3" t="s">
+      <c r="R12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q12" s="3" t="s">
+      <c r="S12" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>95</v>
       </c>
@@ -1764,29 +1858,32 @@
       <c r="I13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="L13" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="N13" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="M13" s="3" t="s">
+      <c r="O13" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="N13" s="3" t="s">
+      <c r="P13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="Q13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P13" s="3" t="s">
+      <c r="R13" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="S13" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>111</v>
       </c>
@@ -1812,28 +1909,31 @@
         <v>20</v>
       </c>
       <c r="J14" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L14" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="M14" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="O14" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="P14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="Q14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P14" s="3" t="s">
+      <c r="R14" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Q14" s="3" t="s">
+      <c r="S14" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>111</v>
       </c>
@@ -1862,31 +1962,37 @@
         <v>19</v>
       </c>
       <c r="J15" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L15" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="N15" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="M15" s="3" t="s">
+      <c r="O15" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="R15" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="S15" s="5" t="s">
+      <c r="U15" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>111</v>
       </c>
@@ -1915,31 +2021,37 @@
         <v>19</v>
       </c>
       <c r="J16" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L16" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="N16" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="M16" s="3" t="s">
+      <c r="O16" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="N16" s="3" t="s">
+      <c r="P16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="R16" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="S16" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>136</v>
       </c>
@@ -1962,34 +2074,40 @@
         <v>19</v>
       </c>
       <c r="J17" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L17" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="O17" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="P17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="R17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="Q17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S17" s="5" t="s">
+      <c r="S17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>136</v>
       </c>
@@ -2015,31 +2133,37 @@
         <v>19</v>
       </c>
       <c r="J18" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L18" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="M18" s="3" t="s">
+      <c r="O18" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="N18" s="3" t="s">
+      <c r="P18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="Q18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="R18" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="Q18" s="3" t="s">
+      <c r="S18" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>157</v>
       </c>
@@ -2065,31 +2189,37 @@
         <v>19</v>
       </c>
       <c r="J19" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L19" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="M19" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="M19" s="3" t="s">
+      <c r="O19" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="N19" s="3" t="s">
+      <c r="P19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="Q19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P19" s="3" t="s">
+      <c r="R19" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="Q19" s="3" t="s">
+      <c r="S19" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>157</v>
       </c>
@@ -2115,34 +2245,40 @@
         <v>19</v>
       </c>
       <c r="J20" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="N20" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="M20" s="3" t="s">
+      <c r="O20" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="N20" s="3" t="s">
+      <c r="P20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O20" s="3" t="s">
+      <c r="Q20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="R20" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="Q20" s="3" t="s">
+      <c r="S20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S20" s="5" t="s">
+      <c r="U20" s="5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>174</v>
       </c>
@@ -2164,32 +2300,35 @@
       <c r="I21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="N21" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="M21" s="3" t="s">
+      <c r="O21" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="P21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O21" s="3" t="s">
+      <c r="Q21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="R21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Q21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S21" s="5" t="s">
+      <c r="S21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U21" s="5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>174</v>
       </c>
@@ -2211,26 +2350,29 @@
       <c r="I22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="K22" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L22" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="M22" s="3" t="s">
+      <c r="O22" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="P22" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="3" t="s">
+      <c r="R22" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>187</v>
       </c>
@@ -2256,34 +2398,40 @@
         <v>19</v>
       </c>
       <c r="J23" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L23" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="N23" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="M23" s="3" t="s">
+      <c r="O23" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="N23" s="3" t="s">
+      <c r="P23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O23" s="3" t="s">
+      <c r="Q23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="R23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Q23" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S23" s="5" t="s">
+      <c r="S23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U23" s="5" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>187</v>
       </c>
@@ -2312,34 +2460,40 @@
         <v>19</v>
       </c>
       <c r="J24" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L24" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="N24" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="O24" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="P24" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O24" s="3" t="s">
+      <c r="Q24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="P24" s="3" t="s">
+      <c r="R24" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="Q24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S24" s="5" t="s">
+      <c r="S24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U24" s="5" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>208</v>
       </c>
@@ -2365,31 +2519,37 @@
         <v>19</v>
       </c>
       <c r="J25" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="L25" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="N25" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="M25" s="3" t="s">
+      <c r="O25" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="N25" s="3" t="s">
+      <c r="P25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="3" t="s">
+      <c r="Q25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="R25" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="Q25" s="3" t="s">
+      <c r="S25" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>208</v>
       </c>
@@ -2412,32 +2572,32 @@
       <c r="I26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="L26" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="N26" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="M26" s="3" t="s">
+      <c r="O26" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="N26" s="3" t="s">
+      <c r="P26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O26" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="R26" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="S26" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="S26" s="5" t="s">
+      <c r="U26" s="5" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>208</v>
       </c>
@@ -2464,31 +2624,37 @@
         <v>19</v>
       </c>
       <c r="J27" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="M27" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="L27" s="3" t="s">
+      <c r="N27" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="M27" s="3" t="s">
+      <c r="O27" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="N27" s="3" t="s">
+      <c r="P27" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P27" s="3" t="s">
+      <c r="R27" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Q27" s="3" t="s">
+      <c r="S27" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>230</v>
       </c>
@@ -2515,31 +2681,37 @@
         <v>19</v>
       </c>
       <c r="J28" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="L28" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="M28" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="N28" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="O28" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="N28" s="3" t="s">
+      <c r="P28" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O28" s="3" t="s">
+      <c r="Q28" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P28" s="3" t="s">
+      <c r="R28" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="Q28" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S28" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>230</v>
       </c>
@@ -2563,38 +2735,94 @@
         <v>20</v>
       </c>
       <c r="J29" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L29" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="N29" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="O29" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="N29" s="3" t="s">
+      <c r="P29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O29" s="3" t="s">
+      <c r="Q29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P29" s="3" t="s">
+      <c r="R29" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="Q29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="S29" s="5" t="s">
+      <c r="S29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U29" s="5" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="L5" twoDigitTextYear="1"/>
+    <ignoredError sqref="N5" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new mice, updates to WCSTP list
</commit_message>
<xml_diff>
--- a/Other_workbooks/wholeCellSTPCellList.xlsx
+++ b/Other_workbooks/wholeCellSTPCellList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="6645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="wb_info" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="609">
   <si>
     <t>Mouse Name</t>
   </si>
@@ -1792,9 +1792,6 @@
     <t>2016_08_04_0014</t>
   </si>
   <si>
-    <t>look at _0014 to _0018 to see the effect of APV, and of light power. I think the dominant factor may be jitter onto the non-RSPY cell (and perhaps not recurrent activity). At 58 Hz, there is a clear difference in STP between HS1 and HS3 (look specifically at _0018)</t>
-  </si>
-  <si>
     <t>CH_160718_B</t>
   </si>
   <si>
@@ -1922,6 +1919,12 @@
   </si>
   <si>
     <t>chronos_gfp</t>
+  </si>
+  <si>
+    <t>look at _0014 to _0018 to see the effect of APV, and of light power. I think the dominant factor may be jitter onto the non-RSPY cell (and perhaps not recurrent activity). At 58 Hz, there is a clear difference in STP between HS1 and HS2 (look specifically at _0018)</t>
+  </si>
+  <si>
+    <t>?_rundown</t>
   </si>
 </sst>
 </file>
@@ -2343,9 +2346,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X88"/>
   <sheetViews>
-    <sheetView showFormulas="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
+    <sheetView showFormulas="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2927,7 +2930,7 @@
         <v>72</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>14</v>
@@ -7156,22 +7159,22 @@
     </row>
     <row r="84" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C84" s="3" t="s">
+      <c r="D84" s="3" t="s">
         <v>566</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="E84" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>568</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>569</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>14</v>
@@ -7195,16 +7198,16 @@
         <v>300</v>
       </c>
       <c r="O84" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="P84" s="3" t="s">
         <v>570</v>
       </c>
-      <c r="P84" s="3" t="s">
+      <c r="Q84" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="Q84" s="3" t="s">
+      <c r="R84" s="3" t="s">
         <v>572</v>
-      </c>
-      <c r="R84" s="3" t="s">
-        <v>573</v>
       </c>
       <c r="S84" s="3" t="s">
         <v>17</v>
@@ -7221,55 +7224,55 @@
     </row>
     <row r="85" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C85" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>576</v>
       </c>
-      <c r="D85" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="E85" s="3" t="s">
+      <c r="G85" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="G85" s="3" t="s">
+      <c r="H85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J85" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="H85" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J85" s="3" t="s">
+      <c r="K85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M85" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="N85" s="3" t="s">
         <v>579</v>
       </c>
-      <c r="K85" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L85" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M85" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="N85" s="3" t="s">
+      <c r="O85" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="O85" s="3" t="s">
+      <c r="P85" s="3" t="s">
         <v>581</v>
       </c>
-      <c r="P85" s="3" t="s">
+      <c r="Q85" s="3" t="s">
         <v>582</v>
       </c>
-      <c r="Q85" s="3" t="s">
+      <c r="R85" s="3" t="s">
         <v>583</v>
-      </c>
-      <c r="R85" s="3" t="s">
-        <v>584</v>
       </c>
       <c r="S85" s="3" t="s">
         <v>17</v>
@@ -7284,24 +7287,24 @@
         <v>482</v>
       </c>
       <c r="X85" s="5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="86" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="D86" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="B86" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C86" s="3" t="s">
+      <c r="E86" s="3" t="s">
         <v>588</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>587</v>
-      </c>
-      <c r="E86" s="3" t="s">
-        <v>589</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>14</v>
@@ -7325,16 +7328,16 @@
         <v>298</v>
       </c>
       <c r="O86" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="P86" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="P86" s="3" t="s">
+      <c r="Q86" s="3" t="s">
         <v>591</v>
       </c>
-      <c r="Q86" s="3" t="s">
+      <c r="R86" s="3" t="s">
         <v>592</v>
-      </c>
-      <c r="R86" s="3" t="s">
-        <v>593</v>
       </c>
       <c r="S86" s="3" t="s">
         <v>17</v>
@@ -7351,7 +7354,7 @@
     </row>
     <row r="87" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>27</v>
@@ -7360,7 +7363,7 @@
         <v>236</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>236</v>
@@ -7384,10 +7387,10 @@
         <v>298</v>
       </c>
       <c r="O87" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="Q87" s="3" t="s">
         <v>599</v>
-      </c>
-      <c r="Q87" s="3" t="s">
-        <v>600</v>
       </c>
       <c r="T87" s="3" t="s">
         <v>56</v>
@@ -7396,57 +7399,57 @@
         <v>124</v>
       </c>
       <c r="X87" s="5" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="88" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D88" s="3" t="s">
         <v>602</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="D88" s="3" t="s">
+      <c r="E88" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="H88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N88" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="O88" s="3" t="s">
         <v>604</v>
-      </c>
-      <c r="H88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="I88" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="K88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="L88" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N88" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="O88" s="3" t="s">
-        <v>605</v>
       </c>
       <c r="Q88" s="3" t="s">
         <v>460</v>
       </c>
       <c r="R88" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="S88" s="3" t="s">
         <v>17</v>
       </c>
       <c r="T88" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="U88" s="3" t="s">
         <v>100</v>
@@ -7468,8 +7471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:XFD54"/>
+    <sheetView topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7848,9 +7851,6 @@
       <c r="D26" s="10">
         <v>1</v>
       </c>
-      <c r="E26" s="10">
-        <v>1</v>
-      </c>
     </row>
     <row r="27" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -8453,11 +8453,11 @@
       <c r="B75" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="C75" s="10">
-        <v>1</v>
-      </c>
-      <c r="E75" s="10">
-        <v>1</v>
+      <c r="C75" s="10" t="s">
+        <v>608</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8562,7 +8562,7 @@
     </row>
     <row r="84" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>14</v>
@@ -8576,7 +8576,7 @@
     </row>
     <row r="85" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>27</v>
@@ -8590,7 +8590,7 @@
     </row>
     <row r="86" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>14</v>
@@ -8604,7 +8604,7 @@
     </row>
     <row r="87" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>27</v>
@@ -8615,7 +8615,7 @@
     </row>
     <row r="88" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>14</v>
@@ -8637,7 +8637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -8742,7 +8742,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>549</v>
       </c>
@@ -8753,49 +8753,49 @@
         <v>563</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>564</v>
+        <v>607</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>594</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>597</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>